<commit_message>
ScoreSystem Improvement and fixed some error bugs
</commit_message>
<xml_diff>
--- a/FengTienPro/Assets/Resources/ExcelFiles/MultiLanguage.xlsx
+++ b/FengTienPro/Assets/Resources/ExcelFiles/MultiLanguage.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elliot\FengTienPro\FengTienVR\FengTienPro\Assets\Resources\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Git\FengTienVR\FengTienPro\Assets\Resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3EC1D2-78EC-445C-BBB6-7DDE45A0D8A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA8C4C6-ECDE-4F9D-BB4E-5785D234F69A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="muitiLang" sheetId="1" r:id="rId1"/>
     <sheet name="trainFeed" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7misnM0AErddeftIyv5/AZ7yUnQmKQ=="/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="300">
   <si>
     <t>id</t>
   </si>
@@ -757,6 +757,2383 @@
   </si>
   <si>
     <t>hint_text</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>goal_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>TalkCanv</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_CheckNasogastricTube</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_TissueClean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>詢問爺爺口味</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>詢問爺爺口味</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_Watch</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_Tap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_Soap</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_WashHandCanv</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_TapClean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_Tissue</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_WashObj</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_CutFish</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_CutVeg</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_InputRice</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_InputWater</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_InputFish</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_InputVeg</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_InputSalt</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_CookFood</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_TasteFood</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_PutOnBib</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_TakeBowl</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_GetTemper</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_TakeSpoon</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_FeedFood</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_FeedWater</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_WashStuff</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_ThrowWaste</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_CleanDesk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_MedsTalk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_GrindMeds</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_MixWater</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_FeedMeds</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_FinishFeedMeds</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>goal_WaterClean</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>脫手表</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>脫手表</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>沾濕雙手</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>沾濕雙手</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>按壓洗手乳</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>按壓洗手乳</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手步驟</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手步驟</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗去泡泡</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗去泡泡</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>衛生紙</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗手</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>衛生紙</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清洗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>廚房物品</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清洗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>廚房物品</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>切魚</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>切魚</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>切菜</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>切菜</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放入米飯</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放入米飯</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>倒入水</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>倒入水</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放入魚肉</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放入魚肉</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放入青菜</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放入青菜</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放入鹽</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>放入鹽</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>適當的時間</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>適當的時間</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>品嘗食物</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>煮飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>品嘗食物</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>圍上圍兜兜</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>圍上圍兜兜</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>拿起粥</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>拿起粥</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>測量粥的溫度</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>測量粥的溫度</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>拿起湯匙</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>拿起湯匙</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食與談話</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食與談話</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>漱口</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵食</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>漱口</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清潔</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清洗廚房用品</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清潔</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清洗廚房用品</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清潔</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>倒掉廚餘</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清潔</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>倒掉廚餘</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清潔</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>擦桌子</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清潔</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>擦桌子</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>談話</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>談話</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>磨藥</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>磨藥</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>混和水</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>混和水</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>確認鼻胃管在胃裡</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>確認鼻胃管在胃裡</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>倒入藥品</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>倒入藥品</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>完成餵藥</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>餵藥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>完成餵藥</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清洗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>擦拭藥物用品</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清洗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>擦拭藥物用品</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清洗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗藥物用品</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(en)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>清洗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>洗藥物用品</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -764,7 +3141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -829,6 +3206,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -850,7 +3233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -866,6 +3249,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1083,8 +3467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1612,55 +3996,397 @@
         <v>195</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A48" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A49" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A50" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A51" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A52" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A53" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A54" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A55" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A56" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A57" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A58" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A59" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A60" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A61" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A62" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A63" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A64" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A65" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A66" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A67" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A68" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A69" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A70" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A71" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A72" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A73" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A74" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A75" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A76" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A77" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A78" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A79" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A80" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A81" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="83" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A83" s="11"/>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="85" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="86" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="87" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="88" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="89" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="90" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="91" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="92" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="93" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="94" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="95" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="96" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="97" ht="15.75" customHeight="1"/>
     <row r="98" ht="15.75" customHeight="1"/>
     <row r="99" ht="15.75" customHeight="1"/>

</xml_diff>